<commit_message>
Day 7 | Final Commit
</commit_message>
<xml_diff>
--- a/Batch/14/Curriculum/Day_7_Data_validation.xlsx
+++ b/Batch/14/Curriculum/Day_7_Data_validation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sunstone\Desktop\accio\Excel\Class Curriculum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\14\Curriculum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCF172E-0F04-4272-B799-5E451DC511DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6942382-3044-4FB2-8040-EEEFC91C5740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="750" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Validation" sheetId="1" r:id="rId1"/>
@@ -209,24 +209,18 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -234,6 +228,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -518,214 +518,214 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="H1" s="3" t="s">
+    <row r="1" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="H1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="4" spans="4:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F4" s="1" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="4" spans="4:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D13" s="4" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="13" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="D13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D14" s="2" t="s">
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>12345</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D15" s="2" t="s">
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="D15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D16" s="2" t="s">
+      <c r="E15" s="1"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="4:12" x14ac:dyDescent="0.45">
+      <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D17" s="2" t="s">
+      <c r="E16" s="1"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.45">
+      <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="22" spans="4:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="D22" s="7" t="s">
+      <c r="E17" s="1"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="22" spans="4:11" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="D22" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D24" s="4" t="s">
+    <row r="24" spans="4:11" x14ac:dyDescent="0.45">
+      <c r="D24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3" t="s">
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="4:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D25" s="2" t="s">
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="4:11" ht="14.55" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="6" t="s">
+      <c r="E25" s="1"/>
+      <c r="F25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="8" t="s">
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="10"/>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D26" s="2" t="s">
+      <c r="J25" s="7"/>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.45">
+      <c r="D26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="8" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="9"/>
-      <c r="K26" s="10"/>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.35">
-      <c r="D27" s="2" t="s">
+      <c r="J26" s="7"/>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.45">
+      <c r="D27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="8" t="s">
+      <c r="E27" s="1"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J27" s="9"/>
-      <c r="K27" s="10"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H1:J2"/>
+    <mergeCell ref="F4:L9"/>
+    <mergeCell ref="F14:H17"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="F25:H27"/>
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="I24:K24"/>
     <mergeCell ref="I25:K25"/>
     <mergeCell ref="I26:K26"/>
     <mergeCell ref="I27:K27"/>
-    <mergeCell ref="H1:J2"/>
-    <mergeCell ref="F4:L9"/>
-    <mergeCell ref="F14:H17"/>
-    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <dataValidations xWindow="528" yWindow="728" count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Error" prompt="Enyter the 5-digit product code_x000a_" sqref="E14:E17" xr:uid="{3CB3F0B6-DCB6-41F9-B9B5-BDFE75E570DF}"/>

</xml_diff>